<commit_message>
Setting Up BrowserActions Class
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/testdata.xlsx
+++ b/src/test/resources/testData/testdata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\POM\src\test\java\org\iti\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\POM\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C04293D2-4037-457F-92B9-E88F1A027191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B2C52E-B7E1-43FB-B7B7-6C6448DEDFEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RegistrationData" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
     <t>5</t>
   </si>
   <si>
-    <t>rtss59@gmail.com</t>
+    <t>ghhhh159@gmail.com</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Creating Locator Abstraction Property file
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/testdata.xlsx
+++ b/src/test/resources/testData/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\POM\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B2C52E-B7E1-43FB-B7B7-6C6448DEDFEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D103BB2-8BEB-4B73-9217-207B56A9D6AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
     <t>5</t>
   </si>
   <si>
-    <t>ghhhh159@gmail.com</t>
+    <t>ahmedrrrrr@gmail.com</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
setting up Headless driver
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/testdata.xlsx
+++ b/src/test/resources/testData/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\POM\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{971AA818-81A7-4AE3-B9B2-56686574FA86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16F1E4D1-002B-45B4-AA31-1D2CAEA02360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,7 +48,7 @@
     <t>5489920</t>
   </si>
   <si>
-    <t>ahmeeeedddddd159@gmail.com</t>
+    <t>ahmedmedhat@testautomation.com</t>
   </si>
 </sst>
 </file>
@@ -393,7 +393,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="22.5703125" customWidth="1"/>
+    <col min="7" max="7" width="37.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Creating DataProvider Class attached to dataProvideClass annotation in testNG
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/testdata.xlsx
+++ b/src/test/resources/testData/testdata.xlsx
@@ -8,18 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\POM\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16F1E4D1-002B-45B4-AA31-1D2CAEA02360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEFB7EDF-1CF7-4F58-B170-5EA2EAFF41D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RegistrationData" sheetId="1" r:id="rId1"/>
+    <sheet name="LoginData" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
@@ -48,7 +59,7 @@
     <t>5489920</t>
   </si>
   <si>
-    <t>ahmedmedhat@testautomation.com</t>
+    <t>ahmed.medhat@testautomation.com</t>
   </si>
 </sst>
 </file>
@@ -387,8 +398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,4 +439,33 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC8254F2-6D4B-4451-94AD-A136E8A12159}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="41.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="str">
+        <f>RegistrationData!G1</f>
+        <v>ahmed.medhat@testautomation.com</v>
+      </c>
+      <c r="B1" t="str">
+        <f>CONCATENATE("'",RegistrationData!H1)</f>
+        <v>'5489920</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>